<commit_message>
Oh Hell yeah !
</commit_message>
<xml_diff>
--- a/BooleanRetrieval/precision-recall-graph.xlsx
+++ b/BooleanRetrieval/precision-recall-graph.xlsx
@@ -4,17 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Precision-Recall Graph" sheetId="5" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ir" localSheetId="0">Data!$A$3:$B$13</definedName>
-    <definedName name="ir_1" localSheetId="0">Data!#REF!</definedName>
-    <definedName name="ir_2" localSheetId="0">Data!#REF!</definedName>
-    <definedName name="ir_3" localSheetId="0">Data!$H$1:$I$11</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -22,31 +19,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ir" type="6" refreshedVersion="3" background="1">
-    <textPr codePage="437" sourceFile="C:\Users\ghff\Desktop\ir.txt" tab="0" comma="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" name="ir1" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\ghff\Desktop\ir.txt" tab="0" comma="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" name="ir2" type="6" refreshedVersion="3" background="1">
-    <textPr codePage="437" sourceFile="C:\Users\ghff\Desktop\ir.txt" tab="0" comma="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" name="ir3" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="1" name="ir1" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\ghff\Desktop\ir.txt" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -176,7 +149,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-IN"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -386,37 +359,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9.1202808970888505E-2</c:v>
+                  <c:v>0.221501881860245</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6821856589936103E-2</c:v>
+                  <c:v>0.221501881860245</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5536142304221802E-2</c:v>
+                  <c:v>0.20657863888904099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.12439281654235E-2</c:v>
+                  <c:v>0.17811684952742901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1911765330801499E-2</c:v>
+                  <c:v>0.16655740079927001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6211098315173501E-2</c:v>
+                  <c:v>0.16290871517195801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4785352396823099E-2</c:v>
+                  <c:v>0.12540428870926501</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3650325641111299E-2</c:v>
+                  <c:v>0.119437441783423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2716353276265099E-2</c:v>
+                  <c:v>0.114918012706467</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1413596681841399E-2</c:v>
+                  <c:v>0.107471131076581</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1365002802602302E-2</c:v>
+                  <c:v>0.107471131076581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,48 +419,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.3739803778885805E-2</c:v>
+                  <c:v>0.247986404777814</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3739803778885805E-2</c:v>
+                  <c:v>0.247986404777814</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8840595144383093E-2</c:v>
+                  <c:v>0.22386302815443801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7720237657724401E-2</c:v>
+                  <c:v>0.20269525433011701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.56598337063695E-2</c:v>
+                  <c:v>0.18258372871300599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3482009209073502E-2</c:v>
+                  <c:v>0.17951744858369101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8667413087486701E-2</c:v>
+                  <c:v>0.12946812224639101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6033195928011801E-2</c:v>
+                  <c:v>0.12187555893814001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5717477758297001E-2</c:v>
+                  <c:v>0.11676554405122</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2758078652841698E-2</c:v>
+                  <c:v>0.11089270367040301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.24181767654218E-2</c:v>
+                  <c:v>0.11057964830471601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="75274880"/>
-        <c:axId val="75285632"/>
+        <c:axId val="77618176"/>
+        <c:axId val="77628544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75274880"/>
+        <c:axId val="77618176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,14 +487,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75285632"/>
+        <c:crossAx val="77628544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75285632"/>
+        <c:axId val="77628544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +520,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75274880"/>
+        <c:crossAx val="77618176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -557,10 +531,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.7854705579110427"/>
-          <c:y val="7.8706879471936636E-2"/>
-          <c:w val="0.20571588253167544"/>
-          <c:h val="0.18443674627624176"/>
+          <c:x val="0.80603553021136698"/>
+          <c:y val="7.8706879471936622E-2"/>
+          <c:w val="0.1851509102313513"/>
+          <c:h val="0.14606781236017127"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -574,7 +548,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -609,11 +583,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ir_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ir" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ir" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D13"/>
+      <selection activeCell="E3" sqref="E3:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -913,11 +883,9 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:5">
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
@@ -930,14 +898,8 @@
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>9.1202808970888505E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,14 +915,8 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>0.1</v>
-      </c>
-      <c r="I2">
-        <v>8.6821856589936103E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -971,19 +927,13 @@
         <v>0.24381863324088501</v>
       </c>
       <c r="D3" s="1">
-        <v>9.1202808970888505E-2</v>
+        <v>0.221501881860245</v>
       </c>
       <c r="E3" s="1">
-        <v>8.3739803778885805E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.2</v>
-      </c>
-      <c r="I3">
-        <v>4.5536142304221802E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.247986404777814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
@@ -994,19 +944,13 @@
         <v>0.24381863324088501</v>
       </c>
       <c r="D4" s="1">
-        <v>8.6821856589936103E-2</v>
+        <v>0.221501881860245</v>
       </c>
       <c r="E4" s="1">
-        <v>8.3739803778885805E-2</v>
-      </c>
-      <c r="H4">
-        <v>0.3</v>
-      </c>
-      <c r="I4">
-        <v>4.12439281654235E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.247986404777814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>0.2</v>
       </c>
@@ -1017,19 +961,13 @@
         <v>0.21670597891989701</v>
       </c>
       <c r="D5" s="1">
-        <v>4.5536142304221802E-2</v>
+        <v>0.20657863888904099</v>
       </c>
       <c r="E5" s="1">
-        <v>6.8840595144383093E-2</v>
-      </c>
-      <c r="H5">
-        <v>0.4</v>
-      </c>
-      <c r="I5">
-        <v>3.1911765330801499E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.22386302815443801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>0.3</v>
       </c>
@@ -1040,19 +978,13 @@
         <v>0.174867953722223</v>
       </c>
       <c r="D6" s="1">
-        <v>4.12439281654235E-2</v>
+        <v>0.17811684952742901</v>
       </c>
       <c r="E6" s="1">
-        <v>4.7720237657724401E-2</v>
-      </c>
-      <c r="H6">
-        <v>0.5</v>
-      </c>
-      <c r="I6">
-        <v>2.6211098315173501E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0.20269525433011701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>0.4</v>
       </c>
@@ -1063,19 +995,13 @@
         <v>0.162786701640971</v>
       </c>
       <c r="D7" s="1">
-        <v>3.1911765330801499E-2</v>
+        <v>0.16655740079927001</v>
       </c>
       <c r="E7" s="1">
-        <v>3.56598337063695E-2</v>
-      </c>
-      <c r="H7">
-        <v>0.6</v>
-      </c>
-      <c r="I7">
-        <v>2.4785352396823099E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0.18258372871300599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>0.5</v>
       </c>
@@ -1086,19 +1012,13 @@
         <v>0.15376644472397499</v>
       </c>
       <c r="D8" s="1">
-        <v>2.6211098315173501E-2</v>
+        <v>0.16290871517195801</v>
       </c>
       <c r="E8" s="1">
-        <v>3.3482009209073502E-2</v>
-      </c>
-      <c r="H8">
-        <v>0.7</v>
-      </c>
-      <c r="I8">
-        <v>2.3650325641111299E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>0.17951744858369101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>0.6</v>
       </c>
@@ -1109,19 +1029,13 @@
         <v>0.13091075009621</v>
       </c>
       <c r="D9" s="1">
-        <v>2.4785352396823099E-2</v>
+        <v>0.12540428870926501</v>
       </c>
       <c r="E9" s="1">
-        <v>2.8667413087486701E-2</v>
-      </c>
-      <c r="H9">
-        <v>0.8</v>
-      </c>
-      <c r="I9">
-        <v>2.2716353276265099E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.12946812224639101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>0.7</v>
       </c>
@@ -1132,19 +1046,13 @@
         <v>0.12672147214646401</v>
       </c>
       <c r="D10" s="1">
-        <v>2.3650325641111299E-2</v>
+        <v>0.119437441783423</v>
       </c>
       <c r="E10" s="1">
-        <v>2.6033195928011801E-2</v>
-      </c>
-      <c r="H10">
-        <v>0.9</v>
-      </c>
-      <c r="I10">
-        <v>2.1413596681841399E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>0.12187555893814001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>0.8</v>
       </c>
@@ -1155,19 +1063,13 @@
         <v>0.124026132706574</v>
       </c>
       <c r="D11" s="1">
-        <v>2.2716353276265099E-2</v>
+        <v>0.114918012706467</v>
       </c>
       <c r="E11" s="1">
-        <v>2.5717477758297001E-2</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>2.1365002802602302E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0.11676554405122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>0.9</v>
       </c>
@@ -1178,13 +1080,13 @@
         <v>0.115761331569621</v>
       </c>
       <c r="D12" s="1">
-        <v>2.1413596681841399E-2</v>
+        <v>0.107471131076581</v>
       </c>
       <c r="E12" s="1">
-        <v>2.2758078652841698E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.11089270367040301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1195,10 +1097,10 @@
         <v>0.11507994059217801</v>
       </c>
       <c r="D13" s="1">
-        <v>2.1365002802602302E-2</v>
+        <v>0.107471131076581</v>
       </c>
       <c r="E13" s="1">
-        <v>2.24181767654218E-2</v>
+        <v>0.11057964830471601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ in the vector space of yore with the normalization of the core ...
</commit_message>
<xml_diff>
--- a/BooleanRetrieval/precision-recall-graph.xlsx
+++ b/BooleanRetrieval/precision-recall-graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -239,37 +239,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.25294294614762097</c:v>
+                  <c:v>0.73653905116585106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25294294614762097</c:v>
+                  <c:v>0.734720869347669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23417895450855</c:v>
+                  <c:v>0.726720869347669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18563501355098699</c:v>
+                  <c:v>0.70549864712544696</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17391510743445901</c:v>
+                  <c:v>0.680215097341897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.163945618494719</c:v>
+                  <c:v>0.66947700210380201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13064428515760099</c:v>
+                  <c:v>0.58250201203219099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.123811063878983</c:v>
+                  <c:v>0.56217381408634604</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.120720366274594</c:v>
+                  <c:v>0.53421701752831596</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11670163788080901</c:v>
+                  <c:v>0.50966259624643095</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.116004576077364</c:v>
+                  <c:v>0.50842283016455903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,37 +299,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.24381863324088501</c:v>
+                  <c:v>0.73170126930228696</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24381863324088501</c:v>
+                  <c:v>0.72988308748410602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21670597891989701</c:v>
+                  <c:v>0.72719336416394798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.174867953722223</c:v>
+                  <c:v>0.70386003083061399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.162786701640971</c:v>
+                  <c:v>0.68179726026784404</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15376644472397499</c:v>
+                  <c:v>0.67100629036817805</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13091075009621</c:v>
+                  <c:v>0.58693483653820999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12672147214646401</c:v>
+                  <c:v>0.56007358177989697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.124026132706574</c:v>
+                  <c:v>0.53343777477644305</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.115761331569621</c:v>
+                  <c:v>0.50660730127306797</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11507994059217801</c:v>
+                  <c:v>0.50548031714608399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,37 +359,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.221501881860245</c:v>
+                  <c:v>0.74313543198619703</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.221501881860245</c:v>
+                  <c:v>0.74113543198619702</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20657863888904099</c:v>
+                  <c:v>0.73446876531952998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17811684952742901</c:v>
+                  <c:v>0.70002432087508604</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16655740079927001</c:v>
+                  <c:v>0.69269098754175196</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16290871517195801</c:v>
+                  <c:v>0.68801252590676898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12540428870926501</c:v>
+                  <c:v>0.58142259850845401</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.119437441783423</c:v>
+                  <c:v>0.54651145318371097</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.114918012706467</c:v>
+                  <c:v>0.52963928012569705</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.107471131076581</c:v>
+                  <c:v>0.50385732055235999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.107471131076581</c:v>
+                  <c:v>0.50368210152858095</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,37 +419,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.247986404777814</c:v>
+                  <c:v>0.619855248036006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.247986404777814</c:v>
+                  <c:v>0.61621888439964201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22386302815443801</c:v>
+                  <c:v>0.61232999551075395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20269525433011701</c:v>
+                  <c:v>0.57600736268756103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18258372871300599</c:v>
+                  <c:v>0.57034069602089399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17951744858369101</c:v>
+                  <c:v>0.56906147524167305</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12946812224639101</c:v>
+                  <c:v>0.46975509395204801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12187555893814001</c:v>
+                  <c:v>0.44457320367430803</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11676554405122</c:v>
+                  <c:v>0.43007156267639701</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11089270367040301</c:v>
+                  <c:v>0.40852024687831501</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11057964830471601</c:v>
+                  <c:v>0.40806047676337198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,11 +457,11 @@
         </c:ser>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="77618176"/>
-        <c:axId val="77628544"/>
+        <c:axId val="83969152"/>
+        <c:axId val="83971456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77618176"/>
+        <c:axId val="83969152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,14 +487,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77628544"/>
+        <c:crossAx val="83971456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77628544"/>
+        <c:axId val="83971456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +520,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77618176"/>
+        <c:crossAx val="83969152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -532,9 +532,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.80603553021136698"/>
-          <c:y val="7.8706879471936622E-2"/>
+          <c:y val="7.8706879471936636E-2"/>
           <c:w val="0.1851509102313513"/>
-          <c:h val="0.14606781236017127"/>
+          <c:h val="0.1460678123601713"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -548,7 +548,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="85" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -921,16 +921,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.25294294614762097</v>
+        <v>0.73653905116585106</v>
       </c>
       <c r="C3" s="1">
-        <v>0.24381863324088501</v>
+        <v>0.73170126930228696</v>
       </c>
       <c r="D3" s="1">
-        <v>0.221501881860245</v>
+        <v>0.74313543198619703</v>
       </c>
       <c r="E3" s="1">
-        <v>0.247986404777814</v>
+        <v>0.619855248036006</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -938,16 +938,16 @@
         <v>0.1</v>
       </c>
       <c r="B4" s="1">
-        <v>0.25294294614762097</v>
+        <v>0.734720869347669</v>
       </c>
       <c r="C4" s="1">
-        <v>0.24381863324088501</v>
+        <v>0.72988308748410602</v>
       </c>
       <c r="D4" s="1">
-        <v>0.221501881860245</v>
+        <v>0.74113543198619702</v>
       </c>
       <c r="E4" s="1">
-        <v>0.247986404777814</v>
+        <v>0.61621888439964201</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -955,16 +955,16 @@
         <v>0.2</v>
       </c>
       <c r="B5" s="1">
-        <v>0.23417895450855</v>
+        <v>0.726720869347669</v>
       </c>
       <c r="C5" s="1">
-        <v>0.21670597891989701</v>
+        <v>0.72719336416394798</v>
       </c>
       <c r="D5" s="1">
-        <v>0.20657863888904099</v>
+        <v>0.73446876531952998</v>
       </c>
       <c r="E5" s="1">
-        <v>0.22386302815443801</v>
+        <v>0.61232999551075395</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -972,16 +972,16 @@
         <v>0.3</v>
       </c>
       <c r="B6" s="1">
-        <v>0.18563501355098699</v>
+        <v>0.70549864712544696</v>
       </c>
       <c r="C6" s="1">
-        <v>0.174867953722223</v>
+        <v>0.70386003083061399</v>
       </c>
       <c r="D6" s="1">
-        <v>0.17811684952742901</v>
+        <v>0.70002432087508604</v>
       </c>
       <c r="E6" s="1">
-        <v>0.20269525433011701</v>
+        <v>0.57600736268756103</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -989,16 +989,16 @@
         <v>0.4</v>
       </c>
       <c r="B7" s="1">
-        <v>0.17391510743445901</v>
+        <v>0.680215097341897</v>
       </c>
       <c r="C7" s="1">
-        <v>0.162786701640971</v>
+        <v>0.68179726026784404</v>
       </c>
       <c r="D7" s="1">
-        <v>0.16655740079927001</v>
+        <v>0.69269098754175196</v>
       </c>
       <c r="E7" s="1">
-        <v>0.18258372871300599</v>
+        <v>0.57034069602089399</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1006,16 +1006,16 @@
         <v>0.5</v>
       </c>
       <c r="B8" s="1">
-        <v>0.163945618494719</v>
+        <v>0.66947700210380201</v>
       </c>
       <c r="C8" s="1">
-        <v>0.15376644472397499</v>
+        <v>0.67100629036817805</v>
       </c>
       <c r="D8" s="1">
-        <v>0.16290871517195801</v>
+        <v>0.68801252590676898</v>
       </c>
       <c r="E8" s="1">
-        <v>0.17951744858369101</v>
+        <v>0.56906147524167305</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1023,16 +1023,16 @@
         <v>0.6</v>
       </c>
       <c r="B9" s="1">
-        <v>0.13064428515760099</v>
+        <v>0.58250201203219099</v>
       </c>
       <c r="C9" s="1">
-        <v>0.13091075009621</v>
+        <v>0.58693483653820999</v>
       </c>
       <c r="D9" s="1">
-        <v>0.12540428870926501</v>
+        <v>0.58142259850845401</v>
       </c>
       <c r="E9" s="1">
-        <v>0.12946812224639101</v>
+        <v>0.46975509395204801</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1040,16 +1040,16 @@
         <v>0.7</v>
       </c>
       <c r="B10" s="1">
-        <v>0.123811063878983</v>
+        <v>0.56217381408634604</v>
       </c>
       <c r="C10" s="1">
-        <v>0.12672147214646401</v>
+        <v>0.56007358177989697</v>
       </c>
       <c r="D10" s="1">
-        <v>0.119437441783423</v>
+        <v>0.54651145318371097</v>
       </c>
       <c r="E10" s="1">
-        <v>0.12187555893814001</v>
+        <v>0.44457320367430803</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1057,16 +1057,16 @@
         <v>0.8</v>
       </c>
       <c r="B11" s="1">
-        <v>0.120720366274594</v>
+        <v>0.53421701752831596</v>
       </c>
       <c r="C11" s="1">
-        <v>0.124026132706574</v>
+        <v>0.53343777477644305</v>
       </c>
       <c r="D11" s="1">
-        <v>0.114918012706467</v>
+        <v>0.52963928012569705</v>
       </c>
       <c r="E11" s="1">
-        <v>0.11676554405122</v>
+        <v>0.43007156267639701</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1074,16 +1074,16 @@
         <v>0.9</v>
       </c>
       <c r="B12" s="1">
-        <v>0.11670163788080901</v>
+        <v>0.50966259624643095</v>
       </c>
       <c r="C12" s="1">
-        <v>0.115761331569621</v>
+        <v>0.50660730127306797</v>
       </c>
       <c r="D12" s="1">
-        <v>0.107471131076581</v>
+        <v>0.50385732055235999</v>
       </c>
       <c r="E12" s="1">
-        <v>0.11089270367040301</v>
+        <v>0.40852024687831501</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1091,16 +1091,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>0.116004576077364</v>
+        <v>0.50842283016455903</v>
       </c>
       <c r="C13" s="1">
-        <v>0.11507994059217801</v>
+        <v>0.50548031714608399</v>
       </c>
       <c r="D13" s="1">
-        <v>0.107471131076581</v>
+        <v>0.50368210152858095</v>
       </c>
       <c r="E13" s="1">
-        <v>0.11057964830471601</v>
+        <v>0.40806047676337198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for Project 2 Phase 2:  - separated local and global query expansions  - for global expansion, add all words in (first) synset  - updated spreadsheet/graph for phase 2
</commit_message>
<xml_diff>
--- a/BooleanRetrieval/precision-recall-graph.xlsx
+++ b/BooleanRetrieval/precision-recall-graph.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Chart1" sheetId="5" r:id="rId2"/>
+    <sheet name="Precision-Recall Graph" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ir" localSheetId="0">Data!$A$3:$B$13</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Recall</t>
   </si>
@@ -50,11 +50,20 @@
   <si>
     <t>Stopwords &amp; Stemming</t>
   </si>
+  <si>
+    <t>Local Query Expansion</t>
+  </si>
+  <si>
+    <t>Global Query Expansion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000000000000000"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -100,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,11 +132,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +154,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -149,7 +173,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-IN"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -236,7 +260,7 @@
             <c:numRef>
               <c:f>Data!$B$3:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.73653905116585106</c:v>
@@ -296,7 +320,7 @@
             <c:numRef>
               <c:f>Data!$C$3:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.73170126930228696</c:v>
@@ -356,7 +380,7 @@
             <c:numRef>
               <c:f>Data!$D$3:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.74313543198619703</c:v>
@@ -416,7 +440,7 @@
             <c:numRef>
               <c:f>Data!$E$3:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.619855248036006</c:v>
@@ -455,13 +479,132 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:hiLowLines/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local Query Expansion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$F$3:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.732385271789875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.730385271789875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72038527178987499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69946607987068299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67983115923576198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67000638980229699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58003490107505395</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55890451558752596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53927062960069805</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51628148212439595</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51628148212439595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Global Query Expansion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$G$3:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.73653905116585106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.734720869347669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.726720869347669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70549864712544696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68063176400856396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66989366877046896</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58569324872342698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56536505077758203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53740825421955296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51019664459508596</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50895687851321403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83969152"/>
-        <c:axId val="83971456"/>
+        <c:axId val="79141888"/>
+        <c:axId val="79152640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83969152"/>
+        <c:axId val="79141888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,14 +630,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83971456"/>
+        <c:crossAx val="79152640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83971456"/>
+        <c:axId val="79152640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,9 +661,9 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83969152"/>
+        <c:crossAx val="79141888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -532,12 +675,17 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.80603553021136698"/>
-          <c:y val="7.8706879471936636E-2"/>
-          <c:w val="0.1851509102313513"/>
-          <c:h val="0.1460678123601713"/>
+          <c:y val="7.0629209173816515E-2"/>
+          <c:w val="0.18649492023208114"/>
+          <c:h val="0.21910171854025684"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -548,7 +696,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -871,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -883,9 +1031,11 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
@@ -898,8 +1048,14 @@
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -915,192 +1071,264 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>0.73653905116585106</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>0.73170126930228696</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>0.74313543198619703</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>0.619855248036006</v>
       </c>
+      <c r="F3" s="5">
+        <v>0.732385271789875</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.73653905116585106</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>0.734720869347669</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>0.72988308748410602</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>0.74113543198619702</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>0.61621888439964201</v>
       </c>
+      <c r="F4" s="5">
+        <v>0.730385271789875</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.734720869347669</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>0.2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>0.726720869347669</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>0.72719336416394798</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>0.73446876531952998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>0.61232999551075395</v>
       </c>
+      <c r="F5" s="5">
+        <v>0.72038527178987499</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.726720869347669</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>0.3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>0.70549864712544696</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>0.70386003083061399</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>0.70002432087508604</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>0.57600736268756103</v>
       </c>
+      <c r="F6" s="5">
+        <v>0.69946607987068299</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.70549864712544696</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>0.4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>0.680215097341897</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>0.68179726026784404</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>0.69269098754175196</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="5">
         <v>0.57034069602089399</v>
       </c>
+      <c r="F7" s="5">
+        <v>0.67983115923576198</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.68063176400856396</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>0.5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>0.66947700210380201</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>0.67100629036817805</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>0.68801252590676898</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="5">
         <v>0.56906147524167305</v>
       </c>
+      <c r="F8" s="5">
+        <v>0.67000638980229699</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.66989366877046896</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>0.6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>0.58250201203219099</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>0.58693483653820999</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>0.58142259850845401</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="5">
         <v>0.46975509395204801</v>
       </c>
+      <c r="F9" s="5">
+        <v>0.58003490107505395</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.58569324872342698</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>0.7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>0.56217381408634604</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="5">
         <v>0.56007358177989697</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>0.54651145318371097</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="5">
         <v>0.44457320367430803</v>
       </c>
+      <c r="F10" s="5">
+        <v>0.55890451558752596</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.56536505077758203</v>
+      </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>0.8</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>0.53421701752831596</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="5">
         <v>0.53343777477644305</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>0.52963928012569705</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="5">
         <v>0.43007156267639701</v>
       </c>
+      <c r="F11" s="5">
+        <v>0.53927062960069805</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.53740825421955296</v>
+      </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>0.9</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>0.50966259624643095</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <v>0.50660730127306797</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="5">
         <v>0.50385732055235999</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="5">
         <v>0.40852024687831501</v>
       </c>
+      <c r="F12" s="5">
+        <v>0.51628148212439595</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.51019664459508596</v>
+      </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>0.50842283016455903</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="5">
         <v>0.50548031714608399</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="5">
         <v>0.50368210152858095</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="5">
         <v>0.40806047676337198</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.51628148212439595</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.50895687851321403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use 3 schemes for Rocchio's algorithm (local query expansion)
</commit_message>
<xml_diff>
--- a/BooleanRetrieval/precision-recall-graph.xlsx
+++ b/BooleanRetrieval/precision-recall-graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Recall</t>
   </si>
@@ -51,10 +51,16 @@
     <t>Stopwords &amp; Stemming</t>
   </si>
   <si>
-    <t>Local Query Expansion</t>
+    <t>Global Query Expansion</t>
   </si>
   <si>
-    <t>Global Query Expansion</t>
+    <t>Local Query Expansion (0.5, 0.5)</t>
+  </si>
+  <si>
+    <t>Local Query Expansion (0.75, 0.25)</t>
+  </si>
+  <si>
+    <t>Local Query Expansion (0.25, 0.75)</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -145,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,14 +159,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +500,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Local Query Expansion</c:v>
+                  <c:v>Local Query Expansion (0.5, 0.5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -503,44 +515,44 @@
                 <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.732385271789875</c:v>
+                  <c:v>0.73983108030702205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.730385271789875</c:v>
+                  <c:v>0.73783108030702205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.72038527178987499</c:v>
+                  <c:v>0.73183108030702204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69946607987068299</c:v>
+                  <c:v>0.709529493005435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67983115923576198</c:v>
+                  <c:v>0.69264060411654604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.67000638980229699</c:v>
+                  <c:v>0.68164060411654603</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58003490107505395</c:v>
+                  <c:v>0.58082115289519698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.55890451558752596</c:v>
+                  <c:v>0.55508147035551503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53927062960069805</c:v>
+                  <c:v>0.54005957058879395</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51628148212439595</c:v>
+                  <c:v>0.51773809171940899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.51628148212439595</c:v>
+                  <c:v>0.51694644528910305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="6"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
@@ -548,7 +560,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Global Query Expansion</c:v>
+                  <c:v>Local Query Expansion (0.25, 0.75)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -563,6 +575,126 @@
                 <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0.73110422765597405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73110422765597405</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71107392462567098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69043756098930797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67623914829089504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67318359273533901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.576404915771496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.549363162838439</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53405683698038897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51136404675022396</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50983932718229796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local Query Expansion (0.75, 0.25)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$H$3:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.732385271789875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.730385271789875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72038527178987499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69946607987068299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67983115923576198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67000638980229699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58003490107505395</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55890451558752596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53927062960069805</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51628148212439595</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51628148212439595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Global Query Expansion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$3:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
                   <c:v>0.73653905116585106</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -600,11 +732,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79141888"/>
-        <c:axId val="79152640"/>
+        <c:axId val="82628992"/>
+        <c:axId val="82631296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79141888"/>
+        <c:axId val="82628992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,14 +762,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79152640"/>
+        <c:crossAx val="82631296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79152640"/>
+        <c:axId val="82631296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +795,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79141888"/>
+        <c:crossAx val="82628992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -674,10 +806,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80603553021136698"/>
-          <c:y val="7.0629209173816515E-2"/>
-          <c:w val="0.18649492023208114"/>
-          <c:h val="0.21910171854025684"/>
+          <c:x val="0.75021631968191604"/>
+          <c:y val="6.0078467888557393E-3"/>
+          <c:w val="0.2497836803180839"/>
+          <c:h val="0.29213562472034249"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -696,7 +828,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1019,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1032,30 +1164,37 @@
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="30">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1077,257 +1216,329 @@
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>0.73653905116585106</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>0.73170126930228696</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>0.74313543198619703</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0.619855248036006</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
+        <v>0.73983108030702205</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.73110422765597405</v>
+      </c>
+      <c r="H3" s="3">
         <v>0.732385271789875</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="3">
         <v>0.73653905116585106</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>0.1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>0.734720869347669</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0.72988308748410602</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.74113543198619702</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0.61621888439964201</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
+        <v>0.73783108030702205</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.73110422765597405</v>
+      </c>
+      <c r="H4" s="3">
         <v>0.730385271789875</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="3">
         <v>0.734720869347669</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>0.2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>0.726720869347669</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0.72719336416394798</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.73446876531952998</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0.61232999551075395</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
+        <v>0.73183108030702204</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.71107392462567098</v>
+      </c>
+      <c r="H5" s="3">
         <v>0.72038527178987499</v>
       </c>
-      <c r="G5" s="5">
+      <c r="I5" s="3">
         <v>0.726720869347669</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>0.3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>0.70549864712544696</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0.70386003083061399</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0.70002432087508604</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0.57600736268756103</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
+        <v>0.709529493005435</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.69043756098930797</v>
+      </c>
+      <c r="H6" s="3">
         <v>0.69946607987068299</v>
       </c>
-      <c r="G6" s="5">
+      <c r="I6" s="3">
         <v>0.70549864712544696</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>0.4</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>0.680215097341897</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>0.68179726026784404</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>0.69269098754175196</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>0.57034069602089399</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
+        <v>0.69264060411654604</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.67623914829089504</v>
+      </c>
+      <c r="H7" s="3">
         <v>0.67983115923576198</v>
       </c>
-      <c r="G7" s="5">
+      <c r="I7" s="3">
         <v>0.68063176400856396</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>0.5</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>0.66947700210380201</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>0.67100629036817805</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>0.68801252590676898</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>0.56906147524167305</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
+        <v>0.68164060411654603</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.67318359273533901</v>
+      </c>
+      <c r="H8" s="3">
         <v>0.67000638980229699</v>
       </c>
-      <c r="G8" s="5">
+      <c r="I8" s="3">
         <v>0.66989366877046896</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>0.6</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>0.58250201203219099</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>0.58693483653820999</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>0.58142259850845401</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>0.46975509395204801</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
+        <v>0.58082115289519698</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.576404915771496</v>
+      </c>
+      <c r="H9" s="3">
         <v>0.58003490107505395</v>
       </c>
-      <c r="G9" s="5">
+      <c r="I9" s="3">
         <v>0.58569324872342698</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>0.7</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>0.56217381408634604</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>0.56007358177989697</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>0.54651145318371097</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>0.44457320367430803</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
+        <v>0.55508147035551503</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.549363162838439</v>
+      </c>
+      <c r="H10" s="3">
         <v>0.55890451558752596</v>
       </c>
-      <c r="G10" s="5">
+      <c r="I10" s="3">
         <v>0.56536505077758203</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>0.8</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>0.53421701752831596</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>0.53343777477644305</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>0.52963928012569705</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>0.43007156267639701</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
+        <v>0.54005957058879395</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.53405683698038897</v>
+      </c>
+      <c r="H11" s="3">
         <v>0.53927062960069805</v>
       </c>
-      <c r="G11" s="5">
+      <c r="I11" s="3">
         <v>0.53740825421955296</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>0.9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>0.50966259624643095</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>0.50660730127306797</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>0.50385732055235999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>0.40852024687831501</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
+        <v>0.51773809171940899</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.51136404675022396</v>
+      </c>
+      <c r="H12" s="3">
         <v>0.51628148212439595</v>
       </c>
-      <c r="G12" s="5">
+      <c r="I12" s="3">
         <v>0.51019664459508596</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>0.50842283016455903</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>0.50548031714608399</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>0.50368210152858095</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>0.40806047676337198</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
+        <v>0.51694644528910305</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.50983932718229796</v>
+      </c>
+      <c r="H13" s="3">
         <v>0.51628148212439595</v>
       </c>
-      <c r="G13" s="5">
+      <c r="I13" s="3">
         <v>0.50895687851321403</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major updates for Project 2 phase 2: - Use part-of-speech resolver (from assignment) - Use recommended WordNet interface - Include query length in vector normalization - Fixed stopwords for stemming+stopwords (read from file rather than relying on null PostingList in index) - Removed document lengths file (was making index incorrect) - Moved stopword and stemming earlier in doVectorQuery function (so query is altered before it is run, so TF is correct)
</commit_message>
<xml_diff>
--- a/BooleanRetrieval/precision-recall-graph.xlsx
+++ b/BooleanRetrieval/precision-recall-graph.xlsx
@@ -8,10 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Precision-Recall Graph" sheetId="5" r:id="rId2"/>
+    <sheet name="Old Data" sheetId="6" r:id="rId2"/>
+    <sheet name="Precision-Recall Graph" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ir" localSheetId="0">Data!$A$3:$B$13</definedName>
+    <definedName name="ir" localSheetId="1">'Old Data'!$A$3:$B$13</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -27,11 +29,19 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="ir11" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\ghff\Desktop\ir.txt" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
   <si>
     <t>Recall</t>
   </si>
@@ -151,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,11 +184,51 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -404,28 +454,28 @@
                   <c:v>0.73446876531952998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70002432087508604</c:v>
+                  <c:v>0.70097670182746696</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69269098754175196</c:v>
+                  <c:v>0.69364336849413299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68801252590676898</c:v>
+                  <c:v>0.68896490685915002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58142259850845401</c:v>
+                  <c:v>0.58237497946083505</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.54651145318371097</c:v>
+                  <c:v>0.54746383413609201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52963928012569705</c:v>
+                  <c:v>0.53059166107807798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50385732055235999</c:v>
+                  <c:v>0.50564303483807505</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.50368210152858095</c:v>
+                  <c:v>0.50546781581429501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,37 +505,37 @@
                 <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.619855248036006</c:v>
+                  <c:v>0.73391980507327703</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61621888439964201</c:v>
+                  <c:v>0.73191980507327703</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.61232999551075395</c:v>
+                  <c:v>0.72358647173994395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57600736268756103</c:v>
+                  <c:v>0.68830869396216598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57034069602089399</c:v>
+                  <c:v>0.68230869396216598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56906147524167305</c:v>
+                  <c:v>0.67626023949265901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46975509395204801</c:v>
+                  <c:v>0.56727331416473703</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44457320367430803</c:v>
+                  <c:v>0.53469613578090702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43007156267639701</c:v>
+                  <c:v>0.51792053665236704</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.40852024687831501</c:v>
+                  <c:v>0.49169667788577898</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.40806047676337198</c:v>
+                  <c:v>0.49169667788577898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,37 +745,37 @@
                 <c:formatCode>0.000000000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.73653905116585106</c:v>
+                  <c:v>0.67689392373980894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.734720869347669</c:v>
+                  <c:v>0.675075741921627</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.726720869347669</c:v>
+                  <c:v>0.667075741921628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70549864712544696</c:v>
+                  <c:v>0.64585351969940497</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68063176400856396</c:v>
+                  <c:v>0.620569969915855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66989366877046896</c:v>
+                  <c:v>0.60983187467776001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58569324872342698</c:v>
+                  <c:v>0.53920118172723897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56536505077758203</c:v>
+                  <c:v>0.51887298378139401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53740825421955296</c:v>
+                  <c:v>0.490916187223364</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51019664459508596</c:v>
+                  <c:v>0.46636176594147899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.50895687851321403</c:v>
+                  <c:v>0.465121999859608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,6 +914,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ir" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ir" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,7 +1208,8 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1237,7 +1292,7 @@
         <v>0.74313543198619703</v>
       </c>
       <c r="E3" s="3">
-        <v>0.619855248036006</v>
+        <v>0.73391980507327703</v>
       </c>
       <c r="F3" s="3">
         <v>0.73983108030702205</v>
@@ -1249,7 +1304,7 @@
         <v>0.732385271789875</v>
       </c>
       <c r="I3" s="3">
-        <v>0.73653905116585106</v>
+        <v>0.67689392373980894</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1266,7 +1321,7 @@
         <v>0.74113543198619702</v>
       </c>
       <c r="E4" s="3">
-        <v>0.61621888439964201</v>
+        <v>0.73191980507327703</v>
       </c>
       <c r="F4" s="3">
         <v>0.73783108030702205</v>
@@ -1278,7 +1333,7 @@
         <v>0.730385271789875</v>
       </c>
       <c r="I4" s="3">
-        <v>0.734720869347669</v>
+        <v>0.675075741921627</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1295,7 +1350,7 @@
         <v>0.73446876531952998</v>
       </c>
       <c r="E5" s="3">
-        <v>0.61232999551075395</v>
+        <v>0.72358647173994395</v>
       </c>
       <c r="F5" s="3">
         <v>0.73183108030702204</v>
@@ -1307,7 +1362,7 @@
         <v>0.72038527178987499</v>
       </c>
       <c r="I5" s="3">
-        <v>0.726720869347669</v>
+        <v>0.667075741921628</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1321,10 +1376,10 @@
         <v>0.70386003083061399</v>
       </c>
       <c r="D6" s="3">
-        <v>0.70002432087508604</v>
+        <v>0.70097670182746696</v>
       </c>
       <c r="E6" s="3">
-        <v>0.57600736268756103</v>
+        <v>0.68830869396216598</v>
       </c>
       <c r="F6" s="3">
         <v>0.709529493005435</v>
@@ -1336,7 +1391,7 @@
         <v>0.69946607987068299</v>
       </c>
       <c r="I6" s="3">
-        <v>0.70549864712544696</v>
+        <v>0.64585351969940497</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1350,10 +1405,10 @@
         <v>0.68179726026784404</v>
       </c>
       <c r="D7" s="3">
-        <v>0.69269098754175196</v>
+        <v>0.69364336849413299</v>
       </c>
       <c r="E7" s="3">
-        <v>0.57034069602089399</v>
+        <v>0.68230869396216598</v>
       </c>
       <c r="F7" s="3">
         <v>0.69264060411654604</v>
@@ -1365,7 +1420,7 @@
         <v>0.67983115923576198</v>
       </c>
       <c r="I7" s="3">
-        <v>0.68063176400856396</v>
+        <v>0.620569969915855</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1379,10 +1434,10 @@
         <v>0.67100629036817805</v>
       </c>
       <c r="D8" s="3">
-        <v>0.68801252590676898</v>
+        <v>0.68896490685915002</v>
       </c>
       <c r="E8" s="3">
-        <v>0.56906147524167305</v>
+        <v>0.67626023949265901</v>
       </c>
       <c r="F8" s="3">
         <v>0.68164060411654603</v>
@@ -1394,7 +1449,7 @@
         <v>0.67000638980229699</v>
       </c>
       <c r="I8" s="3">
-        <v>0.66989366877046896</v>
+        <v>0.60983187467776001</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1408,10 +1463,10 @@
         <v>0.58693483653820999</v>
       </c>
       <c r="D9" s="3">
-        <v>0.58142259850845401</v>
+        <v>0.58237497946083505</v>
       </c>
       <c r="E9" s="3">
-        <v>0.46975509395204801</v>
+        <v>0.56727331416473703</v>
       </c>
       <c r="F9" s="3">
         <v>0.58082115289519698</v>
@@ -1423,7 +1478,7 @@
         <v>0.58003490107505395</v>
       </c>
       <c r="I9" s="3">
-        <v>0.58569324872342698</v>
+        <v>0.53920118172723897</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1437,10 +1492,10 @@
         <v>0.56007358177989697</v>
       </c>
       <c r="D10" s="3">
-        <v>0.54651145318371097</v>
+        <v>0.54746383413609201</v>
       </c>
       <c r="E10" s="3">
-        <v>0.44457320367430803</v>
+        <v>0.53469613578090702</v>
       </c>
       <c r="F10" s="3">
         <v>0.55508147035551503</v>
@@ -1452,7 +1507,7 @@
         <v>0.55890451558752596</v>
       </c>
       <c r="I10" s="3">
-        <v>0.56536505077758203</v>
+        <v>0.51887298378139401</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1466,10 +1521,10 @@
         <v>0.53343777477644305</v>
       </c>
       <c r="D11" s="3">
-        <v>0.52963928012569705</v>
+        <v>0.53059166107807798</v>
       </c>
       <c r="E11" s="3">
-        <v>0.43007156267639701</v>
+        <v>0.51792053665236704</v>
       </c>
       <c r="F11" s="3">
         <v>0.54005957058879395</v>
@@ -1481,7 +1536,7 @@
         <v>0.53927062960069805</v>
       </c>
       <c r="I11" s="3">
-        <v>0.53740825421955296</v>
+        <v>0.490916187223364</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1495,10 +1550,10 @@
         <v>0.50660730127306797</v>
       </c>
       <c r="D12" s="3">
-        <v>0.50385732055235999</v>
+        <v>0.50564303483807505</v>
       </c>
       <c r="E12" s="3">
-        <v>0.40852024687831501</v>
+        <v>0.49169667788577898</v>
       </c>
       <c r="F12" s="3">
         <v>0.51773809171940899</v>
@@ -1510,7 +1565,7 @@
         <v>0.51628148212439595</v>
       </c>
       <c r="I12" s="3">
-        <v>0.51019664459508596</v>
+        <v>0.46636176594147899</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1524,10 +1579,10 @@
         <v>0.50548031714608399</v>
       </c>
       <c r="D13" s="3">
-        <v>0.50368210152858095</v>
+        <v>0.50546781581429501</v>
       </c>
       <c r="E13" s="3">
-        <v>0.40806047676337198</v>
+        <v>0.49169667788577898</v>
       </c>
       <c r="F13" s="3">
         <v>0.51694644528910305</v>
@@ -1539,11 +1594,758 @@
         <v>0.51628148212439595</v>
       </c>
       <c r="I13" s="3">
-        <v>0.50895687851321403</v>
+        <v>0.465121999859608</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.73653905116585106</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.73170126930228696</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.74313543198619703</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.619855248036006</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.73983108030702205</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.73110422765597405</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.732385271789875</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.73653905116585106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.734720869347669</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.72988308748410602</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.74113543198619702</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.61621888439964201</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.73783108030702205</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.73110422765597405</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.730385271789875</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.734720869347669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.726720869347669</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.72719336416394798</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.73446876531952998</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.61232999551075395</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.73183108030702204</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.71107392462567098</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.72038527178987499</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.726720869347669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.70549864712544696</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.70386003083061399</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.70002432087508604</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.57600736268756103</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.709529493005435</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.69043756098930797</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.69946607987068299</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.70549864712544696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.680215097341897</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.68179726026784404</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.69269098754175196</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.57034069602089399</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.69264060411654604</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.67623914829089504</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.67983115923576198</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.68063176400856396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.66947700210380201</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.67100629036817805</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.68801252590676898</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.56906147524167305</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.68164060411654603</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.67318359273533901</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.67000638980229699</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.66989366877046896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.58250201203219099</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.58693483653820999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.58142259850845401</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.46975509395204801</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.58082115289519698</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.576404915771496</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.58003490107505395</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.58569324872342698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.56217381408634604</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.56007358177989697</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.54651145318371097</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.44457320367430803</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.55508147035551503</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.549363162838439</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.55890451558752596</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.56536505077758203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.53421701752831596</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.53343777477644305</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.52963928012569705</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.43007156267639701</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.54005957058879395</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.53405683698038897</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.53927062960069805</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.53740825421955296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.50966259624643095</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.50660730127306797</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.50385732055235999</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.40852024687831501</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.51773809171940899</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.51136404675022396</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.51628148212439595</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.51019664459508596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.50842283016455903</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.50548031714608399</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.50368210152858095</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.40806047676337198</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.51694644528910305</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.50983932718229796</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.51628148212439595</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.50895687851321403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="8">
+        <f>Data!B3-'Old Data'!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <f>Data!C3-'Old Data'!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <f>Data!D3-'Old Data'!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <f>Data!E3-'Old Data'!E3</f>
+        <v>0.11406455703727103</v>
+      </c>
+      <c r="F15" s="8">
+        <f>Data!F3-'Old Data'!F3</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <f>Data!G3-'Old Data'!G3</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <f>Data!H3-'Old Data'!H3</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="8">
+        <f>Data!I3-'Old Data'!I3</f>
+        <v>-5.964512742604211E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="8">
+        <f>Data!B4-'Old Data'!B4</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <f>Data!C4-'Old Data'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <f>Data!D4-'Old Data'!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <f>Data!E4-'Old Data'!E4</f>
+        <v>0.11570092067363502</v>
+      </c>
+      <c r="F16" s="8">
+        <f>Data!F4-'Old Data'!F4</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <f>Data!G4-'Old Data'!G4</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <f>Data!H4-'Old Data'!H4</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <f>Data!I4-'Old Data'!I4</f>
+        <v>-5.9645127426041999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="8">
+        <f>Data!B5-'Old Data'!B5</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <f>Data!C5-'Old Data'!C5</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <f>Data!D5-'Old Data'!D5</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <f>Data!E5-'Old Data'!E5</f>
+        <v>0.11125647622918999</v>
+      </c>
+      <c r="F17" s="8">
+        <f>Data!F5-'Old Data'!F5</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <f>Data!G5-'Old Data'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <f>Data!H5-'Old Data'!H5</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <f>Data!I5-'Old Data'!I5</f>
+        <v>-5.9645127426041E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="8">
+        <f>Data!B6-'Old Data'!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <f>Data!C6-'Old Data'!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="8">
+        <f>Data!D6-'Old Data'!D6</f>
+        <v>9.5238095238092679E-4</v>
+      </c>
+      <c r="E18" s="8">
+        <f>Data!E6-'Old Data'!E6</f>
+        <v>0.11230133127460495</v>
+      </c>
+      <c r="F18" s="8">
+        <f>Data!F6-'Old Data'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <f>Data!G6-'Old Data'!G6</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="8">
+        <f>Data!H6-'Old Data'!H6</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <f>Data!I6-'Old Data'!I6</f>
+        <v>-5.9645127426041999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="8">
+        <f>Data!B7-'Old Data'!B7</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="8">
+        <f>Data!C7-'Old Data'!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <f>Data!D7-'Old Data'!D7</f>
+        <v>9.5238095238103782E-4</v>
+      </c>
+      <c r="E19" s="8">
+        <f>Data!E7-'Old Data'!E7</f>
+        <v>0.11196799794127199</v>
+      </c>
+      <c r="F19" s="8">
+        <f>Data!F7-'Old Data'!F7</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <f>Data!G7-'Old Data'!G7</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
+        <f>Data!H7-'Old Data'!H7</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
+        <f>Data!I7-'Old Data'!I7</f>
+        <v>-6.0061794092708953E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="8">
+        <f>Data!B8-'Old Data'!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="8">
+        <f>Data!C8-'Old Data'!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <f>Data!D8-'Old Data'!D8</f>
+        <v>9.5238095238103782E-4</v>
+      </c>
+      <c r="E20" s="8">
+        <f>Data!E8-'Old Data'!E8</f>
+        <v>0.10719876425098596</v>
+      </c>
+      <c r="F20" s="8">
+        <f>Data!F8-'Old Data'!F8</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <f>Data!G8-'Old Data'!G8</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <f>Data!H8-'Old Data'!H8</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <f>Data!I8-'Old Data'!I8</f>
+        <v>-6.0061794092708953E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="8">
+        <f>Data!B9-'Old Data'!B9</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <f>Data!C9-'Old Data'!C9</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <f>Data!D9-'Old Data'!D9</f>
+        <v>9.5238095238103782E-4</v>
+      </c>
+      <c r="E21" s="8">
+        <f>Data!E9-'Old Data'!E9</f>
+        <v>9.7518220212689022E-2</v>
+      </c>
+      <c r="F21" s="8">
+        <f>Data!F9-'Old Data'!F9</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <f>Data!G9-'Old Data'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
+        <f>Data!H9-'Old Data'!H9</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <f>Data!I9-'Old Data'!I9</f>
+        <v>-4.649206699618802E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="8">
+        <f>Data!B10-'Old Data'!B10</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <f>Data!C10-'Old Data'!C10</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <f>Data!D10-'Old Data'!D10</f>
+        <v>9.5238095238103782E-4</v>
+      </c>
+      <c r="E22" s="8">
+        <f>Data!E10-'Old Data'!E10</f>
+        <v>9.0122932106598996E-2</v>
+      </c>
+      <c r="F22" s="8">
+        <f>Data!F10-'Old Data'!F10</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <f>Data!G10-'Old Data'!G10</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <f>Data!H10-'Old Data'!H10</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <f>Data!I10-'Old Data'!I10</f>
+        <v>-4.649206699618802E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="8">
+        <f>Data!B11-'Old Data'!B11</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <f>Data!C11-'Old Data'!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
+        <f>Data!D11-'Old Data'!D11</f>
+        <v>9.5238095238092679E-4</v>
+      </c>
+      <c r="E23" s="8">
+        <f>Data!E11-'Old Data'!E11</f>
+        <v>8.7848973975970024E-2</v>
+      </c>
+      <c r="F23" s="8">
+        <f>Data!F11-'Old Data'!F11</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <f>Data!G11-'Old Data'!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="8">
+        <f>Data!H11-'Old Data'!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
+        <f>Data!I11-'Old Data'!I11</f>
+        <v>-4.6492066996188963E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="8">
+        <f>Data!B12-'Old Data'!B12</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <f>Data!C12-'Old Data'!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <f>Data!D12-'Old Data'!D12</f>
+        <v>1.7857142857150565E-3</v>
+      </c>
+      <c r="E24" s="8">
+        <f>Data!E12-'Old Data'!E12</f>
+        <v>8.3176431007463969E-2</v>
+      </c>
+      <c r="F24" s="8">
+        <f>Data!F12-'Old Data'!F12</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
+        <f>Data!G12-'Old Data'!G12</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
+        <f>Data!H12-'Old Data'!H12</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <f>Data!I12-'Old Data'!I12</f>
+        <v>-4.3834878653606968E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B15:I24">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>